<commit_message>
Refactored and added Tables
</commit_message>
<xml_diff>
--- a/src/sql/Comp-930/Insert Templates.xlsx
+++ b/src/sql/Comp-930/Insert Templates.xlsx
@@ -12,7 +12,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="4545"/>
   </bookViews>
   <sheets>
-    <sheet name="Add Custome" sheetId="1" r:id="rId1"/>
+    <sheet name="Add Customer" sheetId="1" r:id="rId1"/>
+    <sheet name="Add Invoice" sheetId="2" r:id="rId2"/>
+    <sheet name="Add Product" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Lastname</t>
   </si>
@@ -72,9 +74,6 @@
   </si>
   <si>
     <t>jnsm@email.com</t>
-  </si>
-  <si>
-    <t>(firstname, lastname, address, phone, email)</t>
   </si>
 </sst>
 </file>
@@ -410,18 +409,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G9"/>
+  <dimension ref="A2:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="98.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -443,8 +445,15 @@
       <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="G2" t="str">
+        <f>"insert into customer("&amp;B2&amp;","&amp;C2&amp;","&amp;D2&amp;","&amp;E2&amp;","&amp;F2&amp;")values"</f>
+        <v>insert into customer(Firstname,Lastname,Address,Phone,Email)values</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -461,11 +470,14 @@
         <v>10</v>
       </c>
       <c r="G3" t="str">
-        <f>"insert into customer Values('"&amp;B3&amp;"','"&amp;C3&amp;"','"&amp;D3&amp;"','"&amp;E3&amp;"','"&amp;F3&amp;"')"</f>
-        <v>insert into customer Values('Chisom','Okoye','34 Main Street Calgary','405-678-2354','example@email.com')</v>
+        <f>"('"&amp;B3&amp;"','"&amp;C3&amp;"','"&amp;D3&amp;"','"&amp;E3&amp;"','"&amp;F3&amp;"'),"</f>
+        <v>('Chisom','Okoye','34 Main Street Calgary','405-678-2354','example@email.com'),</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -482,13 +494,159 @@
         <v>15</v>
       </c>
       <c r="G4" t="str">
-        <f>"insert into customer Values('"&amp;B4&amp;"','"&amp;C4&amp;"','"&amp;D4&amp;"','"&amp;E4&amp;"','"&amp;F4&amp;"')"</f>
-        <v>insert into customer Values('John','Smith','45 Adder Lane, Ottawa','613-879-2976','jnsm@email.com')</v>
+        <f>"('"&amp;B4&amp;"','"&amp;C4&amp;"','"&amp;D4&amp;"','"&amp;E4&amp;"','"&amp;F4&amp;"'),"</f>
+        <v>('John','Smith','45 Adder Lane, Ottawa','613-879-2976','jnsm@email.com'),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F5" s="2"/>
+      <c r="G5" t="str">
+        <f t="shared" ref="G5:G29" si="0">"('"&amp;B5&amp;"','"&amp;C5&amp;"','"&amp;D5&amp;"','"&amp;E5&amp;"','"&amp;F5&amp;"'),"</f>
+        <v>('','','','',''),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>('','','','',''),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>('','','','',''),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>('','','','',''),</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>16</v>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>('','','','',''),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>('','','','',''),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>('','','','',''),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v>('','','','',''),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>('','','','',''),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>('','','','',''),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>('','','','',''),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v>('','','','',''),</v>
+      </c>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G17" t="str">
+        <f t="shared" si="0"/>
+        <v>('','','','',''),</v>
+      </c>
+    </row>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G18" t="str">
+        <f t="shared" si="0"/>
+        <v>('','','','',''),</v>
+      </c>
+    </row>
+    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G19" t="str">
+        <f t="shared" si="0"/>
+        <v>('','','','',''),</v>
+      </c>
+    </row>
+    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G20" t="str">
+        <f t="shared" si="0"/>
+        <v>('','','','',''),</v>
+      </c>
+    </row>
+    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G21" t="str">
+        <f t="shared" si="0"/>
+        <v>('','','','',''),</v>
+      </c>
+    </row>
+    <row r="22" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G22" t="str">
+        <f t="shared" si="0"/>
+        <v>('','','','',''),</v>
+      </c>
+    </row>
+    <row r="23" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G23" t="str">
+        <f t="shared" si="0"/>
+        <v>('','','','',''),</v>
+      </c>
+    </row>
+    <row r="24" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G24" t="str">
+        <f t="shared" si="0"/>
+        <v>('','','','',''),</v>
+      </c>
+    </row>
+    <row r="25" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G25" t="str">
+        <f t="shared" si="0"/>
+        <v>('','','','',''),</v>
+      </c>
+    </row>
+    <row r="26" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G26" t="str">
+        <f t="shared" si="0"/>
+        <v>('','','','',''),</v>
+      </c>
+    </row>
+    <row r="27" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G27" t="str">
+        <f t="shared" si="0"/>
+        <v>('','','','',''),</v>
+      </c>
+    </row>
+    <row r="28" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G28" t="str">
+        <f t="shared" si="0"/>
+        <v>('','','','',''),</v>
+      </c>
+    </row>
+    <row r="29" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G29" t="str">
+        <f t="shared" si="0"/>
+        <v>('','','','',''),</v>
       </c>
     </row>
   </sheetData>
@@ -498,4 +656,32 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Building Templates for Populating DB
</commit_message>
<xml_diff>
--- a/src/sql/Comp-930/Insert Templates.xlsx
+++ b/src/sql/Comp-930/Insert Templates.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="4545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="4545" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Add Customer" sheetId="1" r:id="rId1"/>
     <sheet name="Add Invoice" sheetId="2" r:id="rId2"/>
     <sheet name="Add Product" sheetId="3" r:id="rId3"/>
+    <sheet name="Item" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>Lastname</t>
   </si>
@@ -74,6 +75,36 @@
   </si>
   <si>
     <t>jnsm@email.com</t>
+  </si>
+  <si>
+    <t>Customer ID</t>
+  </si>
+  <si>
+    <t>Order Date</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>02/01/2020</t>
+  </si>
+  <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>Product Description</t>
+  </si>
+  <si>
+    <t>Unit Price</t>
+  </si>
+  <si>
+    <t>Total Stock</t>
+  </si>
+  <si>
+    <t>Invoice ID</t>
+  </si>
+  <si>
+    <t>Product ID</t>
   </si>
 </sst>
 </file>
@@ -411,8 +442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,28 +691,946 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:E103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="str">
+        <f>"insert into invoice("&amp;B2&amp;","&amp;C2&amp;","&amp;D2&amp;")values"</f>
+        <v>insert into invoice(Customer ID,Order Date,Total)values</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3">
+        <v>20.67</v>
+      </c>
+      <c r="E3" s="2" t="str">
+        <f>"('"&amp;B3&amp;"','"&amp;C3&amp;"','"&amp;D3&amp;"'),"</f>
+        <v>('1','02/01/2020','20.67'),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="B50">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>61</v>
+      </c>
+      <c r="B63">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="B64">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>63</v>
+      </c>
+      <c r="B65">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>64</v>
+      </c>
+      <c r="B66">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>65</v>
+      </c>
+      <c r="B67">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>66</v>
+      </c>
+      <c r="B68">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>67</v>
+      </c>
+      <c r="B69">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>68</v>
+      </c>
+      <c r="B70">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>69</v>
+      </c>
+      <c r="B71">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>70</v>
+      </c>
+      <c r="B72">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>71</v>
+      </c>
+      <c r="B73">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>72</v>
+      </c>
+      <c r="B74">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>73</v>
+      </c>
+      <c r="B75">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>74</v>
+      </c>
+      <c r="B76">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>75</v>
+      </c>
+      <c r="B77">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>76</v>
+      </c>
+      <c r="B78">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>77</v>
+      </c>
+      <c r="B79">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>78</v>
+      </c>
+      <c r="B80">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>79</v>
+      </c>
+      <c r="B81">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>80</v>
+      </c>
+      <c r="B82">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>81</v>
+      </c>
+      <c r="B83">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>82</v>
+      </c>
+      <c r="B84">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>83</v>
+      </c>
+      <c r="B85">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>84</v>
+      </c>
+      <c r="B86">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>85</v>
+      </c>
+      <c r="B87">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>86</v>
+      </c>
+      <c r="B88">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>87</v>
+      </c>
+      <c r="B89">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>88</v>
+      </c>
+      <c r="B90">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>89</v>
+      </c>
+      <c r="B91">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>90</v>
+      </c>
+      <c r="B92">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>91</v>
+      </c>
+      <c r="B93">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>92</v>
+      </c>
+      <c r="B94">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>93</v>
+      </c>
+      <c r="B95">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>94</v>
+      </c>
+      <c r="B96">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>95</v>
+      </c>
+      <c r="B97">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>96</v>
+      </c>
+      <c r="B98">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>97</v>
+      </c>
+      <c r="B99">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>98</v>
+      </c>
+      <c r="B100">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>99</v>
+      </c>
+      <c r="B101">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>100</v>
+      </c>
+      <c r="B102">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>101</v>
+      </c>
+      <c r="B103">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="5.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="str">
+        <f>"insert into product("&amp;B2&amp;","&amp;C2&amp;","&amp;D2&amp;",'"&amp;E2&amp;"')values"</f>
+        <v>insert into product(Product Name,Product Description,Unit Price,'Total Stock')values</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="str">
+        <f>"insert into item('"&amp;B2&amp;"',"&amp;C2&amp;","&amp;D2&amp;","&amp;E2&amp;",'"&amp;F2&amp;"')values"</f>
+        <v>insert into item('Invoice ID',Product ID,Product Name,Unit Price,'Total')values</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>